<commit_message>
posição das colunas por expressao regular y = bs_html.find_all('div', style=re.compile(r'left:28[0-5]px.*?top:314px'))
</commit_message>
<xml_diff>
--- a/notas/Pasta1.xlsx
+++ b/notas/Pasta1.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudio\Documents\Python\ETL_PDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudio\Documents\Python\ETL_PDF\notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="11955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$4:$O$45</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="106">
   <si>
     <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;</t>
   </si>
@@ -312,6 +313,39 @@
   </si>
   <si>
     <t>Interc. Internacional</t>
+  </si>
+  <si>
+    <t>&lt;/div</t>
+  </si>
+  <si>
+    <t>Sábado, 11 Junho de 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:419px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:189px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:150px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> height:11px</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>391px; top</t>
+  </si>
+  <si>
+    <t>189px; width</t>
+  </si>
+  <si>
+    <t>178px; height</t>
+  </si>
+  <si>
+    <t>11px;"&gt;</t>
   </si>
 </sst>
 </file>
@@ -926,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,4 +2919,72 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extraindo os dados do objeto beautifulsoup via regex
</commit_message>
<xml_diff>
--- a/notas/Pasta1.xlsx
+++ b/notas/Pasta1.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="11955"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="resumo_balanço" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$4:$O$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">resumo_balanço!$A$4:$O$45</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="147">
   <si>
     <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;</t>
   </si>
@@ -346,6 +347,129 @@
   </si>
   <si>
     <t>11px;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:32px; top:456px; width:420px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Produção e Carga por Submercados e Intercâmbios Verificados - MWmed</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:109px; top:483px; width:31px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Norte</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:49px; top:505px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:49px; top:522px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:49px; top:538px; width:45px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*)</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:171px; top:505px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;4.320</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:171px; top:521px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;1.677</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:171px; top:538px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;5.438</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:75px; top:571px; width:96px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Itaipu Binacional</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:222px; top:494px; width:18px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;559</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:324px; top:494px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;3.270</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:443px; top:482px; width:52px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Nordeste</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:504px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:521px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:309px; top:547px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;2.711</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:538px; width:32px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Eólica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:554px; width:49px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*) </t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:519px; top:504px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;2.589</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:519px; top:521px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;2.324</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:519px; top:537px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;1.917</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:513px; top:554px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;10.100</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:219px; top:605px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;11.361</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:275px; top:643px; width:18px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Sul</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:407px; top:584px; width:126px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Sudeste/Centro-Oeste</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:390px; top:606px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:390px; top:622px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:390px; top:639px; width:45px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*)</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:512px; top:606px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;19.233</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:518px; top:621px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;5.092</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:512px; top:638px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;34.895</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:145px; top:660px; width:22px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;-643</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:213px; top:665px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:324px; top:666px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;11.837</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:57px; top:696px; width:114px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Interc. Internacional</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:213px; top:682px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:213px; top:698px; width:32px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Eólica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:214px; top:714px; width:49px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*) </t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:340px; top:683px; width:18px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;836</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:340px; top:699px; width:18px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;576</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:324px; top:716px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;10.686</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:404px; top:682px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;1.920</t>
   </si>
 </sst>
 </file>
@@ -960,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2925,7 +3049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2987,4 +3111,224 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agora com  o dicionário de texto organizado
</commit_message>
<xml_diff>
--- a/notas/Pasta1.xlsx
+++ b/notas/Pasta1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="resumo_balanço" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
+    <sheet name="resumo_por_subsis" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">resumo_balanço!$A$4:$O$45</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="179">
   <si>
     <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;</t>
   </si>
@@ -349,127 +349,223 @@
     <t>11px;"&gt;</t>
   </si>
   <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:32px; top:456px; width:420px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Produção e Carga por Submercados e Intercâmbios Verificados - MWmed</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:109px; top:483px; width:31px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Norte</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:49px; top:505px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:49px; top:522px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:49px; top:538px; width:45px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*)</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:171px; top:505px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;4.320</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:171px; top:521px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;1.677</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:171px; top:538px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;5.438</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:75px; top:571px; width:96px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Itaipu Binacional</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:222px; top:494px; width:18px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;559</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:324px; top:494px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;3.270</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:443px; top:482px; width:52px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Nordeste</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:504px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:521px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:309px; top:547px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;2.711</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:538px; width:32px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Eólica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:391px; top:554px; width:49px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*) </t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:519px; top:504px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;2.589</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:519px; top:521px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;2.324</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:519px; top:537px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;1.917</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:513px; top:554px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;10.100</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:219px; top:605px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;11.361</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:275px; top:643px; width:18px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Sul</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:407px; top:584px; width:126px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Sudeste/Centro-Oeste</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:390px; top:606px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:390px; top:622px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:390px; top:639px; width:45px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*)</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:512px; top:606px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;19.233</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:518px; top:621px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;5.092</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:512px; top:638px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;34.895</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:145px; top:660px; width:22px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;-643</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:213px; top:665px; width:82px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Hidro</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:324px; top:666px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;11.837</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:57px; top:696px; width:114px; height:11px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:11px"&gt;Interc. Internacional</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:213px; top:682px; width:106px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Produção Termo (**)</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:213px; top:698px; width:32px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Eólica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:214px; top:714px; width:49px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;Carga (*) </t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:340px; top:683px; width:18px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;836</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:340px; top:699px; width:18px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;576</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:324px; top:716px; width:33px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;10.686</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div style="position:absolute; border: textbox 1px solid; writing-mode:lr-tb; left:404px; top:682px; width:27px; height:10px;"&gt;&lt;span style="font-family: Arial-BoldMT; font-size:10px"&gt;1.920</t>
+    <t>&lt;br</t>
+  </si>
+  <si>
+    <t>&lt;/span</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:32px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:456px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:420px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:109px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:483px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:31px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:49px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:505px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:82px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> height:10px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:522px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:106px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:538px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:45px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:171px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:27px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:521px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:75px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:571px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:96px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:222px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:494px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:18px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:324px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:443px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:482px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:52px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:391px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:504px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:309px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:547px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:32px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:554px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:49px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:519px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:537px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:513px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:33px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:219px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:605px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:275px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:643px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:407px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:584px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:126px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:390px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:606px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:622px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:639px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:512px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:518px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:621px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:638px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:145px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:660px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:22px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:213px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:665px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:666px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:57px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:696px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> width:114px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:682px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:698px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:214px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:714px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:340px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:683px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:699px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> top:716px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> left:404px</t>
   </si>
 </sst>
 </file>
@@ -713,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -768,6 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,7 +1182,7 @@
   <dimension ref="A4:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D13" sqref="D13:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,217 +3212,1454 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A41"/>
+      <selection activeCell="G2" sqref="G2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="54">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="54">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="54">
+        <v>5438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" s="54">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" t="s">
+        <v>117</v>
+      </c>
+      <c r="L15" s="54">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="I16" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17" t="s">
+        <v>141</v>
+      </c>
+      <c r="J17" t="s">
+        <v>117</v>
+      </c>
+      <c r="L17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="54">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" t="s">
+        <v>117</v>
+      </c>
+      <c r="L19" s="54">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" t="s">
+        <v>117</v>
+      </c>
+      <c r="L20" s="54">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" t="s">
+        <v>145</v>
+      </c>
+      <c r="J21" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21" s="54">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>146</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" t="s">
+        <v>145</v>
+      </c>
+      <c r="J22" t="s">
+        <v>117</v>
+      </c>
+      <c r="L22" s="54">
+        <v>11361</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H23" t="s">
+        <v>149</v>
+      </c>
+      <c r="I23" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" t="s">
+        <v>152</v>
+      </c>
+      <c r="J24" t="s">
+        <v>100</v>
+      </c>
+      <c r="L24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>153</v>
+      </c>
+      <c r="H25" t="s">
+        <v>154</v>
+      </c>
+      <c r="I25" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" t="s">
+        <v>117</v>
+      </c>
+      <c r="L25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26" t="s">
+        <v>155</v>
+      </c>
+      <c r="I26" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26" t="s">
+        <v>117</v>
+      </c>
+      <c r="L26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="J27" t="s">
+        <v>117</v>
+      </c>
+      <c r="L27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>157</v>
+      </c>
+      <c r="H28" t="s">
+        <v>154</v>
+      </c>
+      <c r="I28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J28" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" s="54">
+        <v>19233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" t="s">
+        <v>159</v>
+      </c>
+      <c r="I29" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="J29" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" s="54">
+        <v>5092</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>157</v>
+      </c>
+      <c r="H30" t="s">
+        <v>160</v>
+      </c>
+      <c r="I30" t="s">
+        <v>145</v>
+      </c>
+      <c r="J30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" s="54">
+        <v>34895</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" t="s">
+        <v>162</v>
+      </c>
+      <c r="I31" t="s">
+        <v>163</v>
+      </c>
+      <c r="J31" t="s">
+        <v>117</v>
+      </c>
+      <c r="L31">
+        <v>-643</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>164</v>
+      </c>
+      <c r="H32" t="s">
+        <v>165</v>
+      </c>
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
+      <c r="J32" t="s">
+        <v>117</v>
+      </c>
+      <c r="L32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" t="s">
+        <v>166</v>
+      </c>
+      <c r="I33" t="s">
+        <v>145</v>
+      </c>
+      <c r="J33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L33" s="54">
+        <v>11837</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" t="s">
+        <v>169</v>
+      </c>
+      <c r="J34" t="s">
+        <v>100</v>
+      </c>
+      <c r="L34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>164</v>
+      </c>
+      <c r="H35" t="s">
+        <v>170</v>
+      </c>
+      <c r="I35" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" t="s">
+        <v>117</v>
+      </c>
+      <c r="L35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>164</v>
+      </c>
+      <c r="H36" t="s">
+        <v>171</v>
+      </c>
+      <c r="I36" t="s">
+        <v>139</v>
+      </c>
+      <c r="J36" t="s">
+        <v>117</v>
+      </c>
+      <c r="L36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>172</v>
+      </c>
+      <c r="H37" t="s">
+        <v>173</v>
+      </c>
+      <c r="I37" t="s">
+        <v>141</v>
+      </c>
+      <c r="J37" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" t="s">
+        <v>175</v>
+      </c>
+      <c r="I38" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="J38" t="s">
+        <v>117</v>
+      </c>
+      <c r="L38">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>174</v>
+      </c>
+      <c r="H39" t="s">
+        <v>176</v>
+      </c>
+      <c r="I39" t="s">
+        <v>130</v>
+      </c>
+      <c r="J39" t="s">
+        <v>117</v>
+      </c>
+      <c r="L39">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="H40" t="s">
+        <v>177</v>
+      </c>
+      <c r="I40" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>117</v>
+      </c>
+      <c r="L40" s="54">
+        <v>10686</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>178</v>
+      </c>
+      <c r="H41" t="s">
+        <v>170</v>
+      </c>
+      <c r="I41" t="s">
+        <v>123</v>
+      </c>
+      <c r="J41" t="s">
+        <v>117</v>
+      </c>
+      <c r="L41" s="54">
+        <v>1920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>